<commit_message>
2 sheet for the JDB and add idea on use-case
un fichier excel avec deux feuilles pour le journal de bord
</commit_message>
<xml_diff>
--- a/DOC/Quentin_JDB.xlsx
+++ b/DOC/Quentin_JDB.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Quentin" sheetId="1" r:id="rId1"/>
+    <sheet name="Philippe" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$E$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Quentin!$A$1:$E$37</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -790,8 +791,8 @@
   </sheetPr>
   <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,4 +1513,731 @@
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="68" fitToHeight="5" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H122"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="22"/>
+    <col min="2" max="2" width="9.5703125" style="31" customWidth="1"/>
+    <col min="3" max="3" width="75.28515625" customWidth="1"/>
+    <col min="4" max="4" width="44" customWidth="1"/>
+    <col min="5" max="5" width="42.42578125" customWidth="1"/>
+    <col min="6" max="6" width="58.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="45"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="22"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="22"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="51">
+        <f>SUM(B8:B13)</f>
+        <v>0.10069444444444445</v>
+      </c>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="34"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="49">
+        <v>43343</v>
+      </c>
+      <c r="B8" s="48">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="50"/>
+      <c r="B9" s="25">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="50"/>
+      <c r="B10" s="24">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="50"/>
+      <c r="B11" s="24">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="50"/>
+      <c r="B12" s="24">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="50"/>
+      <c r="B13" s="21">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="27">
+        <f>SUM(B15:B23)</f>
+        <v>0.1875</v>
+      </c>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="34"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="35">
+        <v>43347</v>
+      </c>
+      <c r="B15" s="30">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="36"/>
+      <c r="B16" s="24">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="14"/>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="36"/>
+      <c r="B17" s="24">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="14"/>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="36"/>
+      <c r="B18" s="24">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="38">
+        <v>43350</v>
+      </c>
+      <c r="B19" s="30">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="38"/>
+      <c r="B20" s="30">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="38"/>
+      <c r="B21" s="30">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="38"/>
+      <c r="B22" s="30">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="39"/>
+      <c r="B23" s="24">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="29"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="34"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="35"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="14"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="36"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="14"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="36"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="14"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="36"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="14"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="37"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="20"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="40"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="41"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+      <c r="B34"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35"/>
+      <c r="B35"/>
+    </row>
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36"/>
+      <c r="B36"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+      <c r="B37"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38"/>
+      <c r="B38"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39"/>
+      <c r="B39"/>
+    </row>
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40"/>
+      <c r="B40"/>
+    </row>
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41"/>
+      <c r="B41"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42"/>
+      <c r="B42"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43"/>
+      <c r="B43"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44"/>
+      <c r="B44"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45"/>
+      <c r="B45"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46"/>
+      <c r="B46"/>
+    </row>
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47"/>
+      <c r="B47"/>
+    </row>
+    <row r="48" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48"/>
+      <c r="B48"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49"/>
+      <c r="B49"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50"/>
+      <c r="B50"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51"/>
+      <c r="B51"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52"/>
+      <c r="B52"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53"/>
+      <c r="B53"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54"/>
+      <c r="B54"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55"/>
+      <c r="B55"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56"/>
+      <c r="B56"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57"/>
+      <c r="B57"/>
+    </row>
+    <row r="58" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58"/>
+      <c r="B58"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59"/>
+      <c r="B59"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60"/>
+      <c r="B60"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61"/>
+      <c r="B61"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62"/>
+      <c r="B62"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63"/>
+      <c r="B63"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64"/>
+      <c r="B64"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65"/>
+      <c r="B65"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66"/>
+      <c r="B66"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67"/>
+      <c r="B67"/>
+    </row>
+    <row r="68" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68"/>
+      <c r="B68"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69"/>
+      <c r="B69"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70"/>
+      <c r="B70"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71"/>
+      <c r="B71"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72"/>
+      <c r="B72"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73"/>
+      <c r="B73"/>
+    </row>
+    <row r="74" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74"/>
+      <c r="B74"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75"/>
+      <c r="B75"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76"/>
+      <c r="B76"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77"/>
+      <c r="B77"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78"/>
+      <c r="B78"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79"/>
+      <c r="B79"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80"/>
+      <c r="B80"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81"/>
+      <c r="B81"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82"/>
+      <c r="B82"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83"/>
+      <c r="B83"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84"/>
+      <c r="B84"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85"/>
+      <c r="B85"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86"/>
+      <c r="B86"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87"/>
+      <c r="B87"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88"/>
+      <c r="B88"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89"/>
+      <c r="B89"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90"/>
+      <c r="B90"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91"/>
+      <c r="B91"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92"/>
+      <c r="B92"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93"/>
+      <c r="B93"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94"/>
+      <c r="B94"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95"/>
+      <c r="B95"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96"/>
+      <c r="B96"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97"/>
+      <c r="B97"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98"/>
+      <c r="B98"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99"/>
+      <c r="B99"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100"/>
+      <c r="B100"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101"/>
+      <c r="B101"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102"/>
+      <c r="B102"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103"/>
+      <c r="B103"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104"/>
+      <c r="B104"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105"/>
+      <c r="B105"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106"/>
+      <c r="B106"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107"/>
+      <c r="B107"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108"/>
+      <c r="B108"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109"/>
+      <c r="B109"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110"/>
+      <c r="B110"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111"/>
+      <c r="B111"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112"/>
+      <c r="B112"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113"/>
+      <c r="B113"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114"/>
+      <c r="B114"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115"/>
+      <c r="B115"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116"/>
+      <c r="B116"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117"/>
+      <c r="B117"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118"/>
+      <c r="B118"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119"/>
+      <c r="B119"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120"/>
+      <c r="B120"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121"/>
+      <c r="B121"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122"/>
+      <c r="B122"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout du jour d'aujourd'hui
</commit_message>
<xml_diff>
--- a/DOC/Quentin_JDB.xlsx
+++ b/DOC/Quentin_JDB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Quentin" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -119,6 +119,24 @@
   </si>
   <si>
     <t>Commencement de l'écriture des uses-case et scénario</t>
+  </si>
+  <si>
+    <t>Présentation de Mme. Rappopo sur le coté soin du CPNV et administratif par M.Chevillaz</t>
+  </si>
+  <si>
+    <t>Explication des deux maquettes</t>
+  </si>
+  <si>
+    <t>Discution avec Philipe sur le CDC, la maquette et les scénarios, répartition des tâches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecriture des scénarios </t>
+  </si>
+  <si>
+    <t>Relecture du CDC et ajout / réecriture / suppression de différentes parties</t>
+  </si>
+  <si>
+    <t>Certains points ne sont pas claire, ou innutile, ou manquant. Essayons de prendre le point de vue le plus claire et utile pour le client</t>
   </si>
 </sst>
 </file>
@@ -337,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -349,9 +367,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -416,6 +431,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -425,56 +482,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -789,28 +810,28 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H122"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="22"/>
-    <col min="2" max="2" width="9.5703125" style="31" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="21"/>
+    <col min="2" max="2" width="9.5703125" style="30" customWidth="1"/>
     <col min="3" max="3" width="75.28515625" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
     <col min="5" max="5" width="42.42578125" customWidth="1"/>
     <col min="6" max="6" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="41"/>
       <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
@@ -818,10 +839,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="47"/>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="42"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
@@ -829,25 +850,25 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="22"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="22"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="21"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="21"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -860,286 +881,314 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="51">
+      <c r="B7" s="32">
         <f>SUM(B8:B13)</f>
         <v>0.10069444444444445</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="49">
+      <c r="C7" s="45"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="47"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="48">
         <v>43343</v>
       </c>
-      <c r="B8" s="48">
+      <c r="B8" s="31">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="14"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="25">
+      <c r="D8" s="10"/>
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="49"/>
+      <c r="B9" s="24">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="14" t="s">
+      <c r="D9" s="10"/>
+      <c r="E9" s="13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="24">
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="49"/>
+      <c r="B10" s="23">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="24">
+      <c r="D10" s="10"/>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="49"/>
+      <c r="B11" s="23">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="14"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="24">
+      <c r="D11" s="10"/>
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="49"/>
+      <c r="B12" s="23">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="14"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50"/>
-      <c r="B13" s="21">
+      <c r="D12" s="10"/>
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="49"/>
+      <c r="B13" s="20">
         <v>3.125E-2</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="14"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="29" t="s">
+      <c r="D13" s="11"/>
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="26">
         <f>SUM(B15:B23)</f>
         <v>0.1875</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="34"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="45"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="47"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35">
         <v>43347</v>
       </c>
-      <c r="B15" s="30">
+      <c r="B15" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="14" t="s">
+      <c r="D15" s="10"/>
+      <c r="E15" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
-      <c r="B16" s="24">
+      <c r="B16" s="23">
         <v>3.4722222222222224E-2</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="14"/>
-      <c r="G16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="13"/>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="36"/>
-      <c r="B17" s="24">
+      <c r="B17" s="23">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="14"/>
-      <c r="G17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="13"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
-      <c r="B18" s="24">
+      <c r="B18" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="14" t="s">
+      <c r="D18" s="10"/>
+      <c r="E18" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="38">
+      <c r="A19" s="37">
         <v>43350</v>
       </c>
-      <c r="B19" s="30">
+      <c r="B19" s="29">
         <v>3.125E-2</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="14"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
-      <c r="B20" s="30">
+      <c r="A20" s="37"/>
+      <c r="B20" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="14" t="s">
+      <c r="D20" s="10"/>
+      <c r="E20" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="30">
+      <c r="A21" s="37"/>
+      <c r="B21" s="29">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="14"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="30">
+      <c r="A22" s="37"/>
+      <c r="B22" s="29">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="14"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="39"/>
-      <c r="B23" s="24">
+      <c r="A23" s="38"/>
+      <c r="B23" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="15"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="14"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="29"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="34"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="14"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="26">
+        <f>SUM(B25:B29)</f>
+        <v>9.375E-2</v>
+      </c>
+      <c r="C24" s="45"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="47"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="35">
+        <v>43354</v>
+      </c>
+      <c r="B25" s="24">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="16"/>
+      <c r="E25" s="13"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="14"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="24">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="16"/>
+      <c r="E26" s="13"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="36"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="14"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
+      <c r="B27" s="24">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="14"/>
+      <c r="B28" s="24">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="15"/>
+      <c r="E28" s="50"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="37"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="20"/>
-      <c r="G29" s="10"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="25">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="17"/>
+      <c r="E29" s="51"/>
+      <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="40"/>
+      <c r="D30" s="33"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="41"/>
+      <c r="D31" s="34"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32"/>
-      <c r="C32" s="11"/>
+      <c r="C32" s="10"/>
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33"/>
       <c r="B33"/>
-      <c r="C33" s="11"/>
+      <c r="C33" s="10"/>
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1499,16 +1548,17 @@
       <c r="B122"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="D30:D31"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A19:A23"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="A8:A13"/>
+    <mergeCell ref="E27:E29"/>
     <mergeCell ref="A25:A29"/>
     <mergeCell ref="C24:E24"/>
-    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="68" fitToHeight="5" orientation="landscape" r:id="rId1"/>
@@ -1519,14 +1569,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="22"/>
-    <col min="2" max="2" width="9.5703125" style="31" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="21"/>
+    <col min="2" max="2" width="9.5703125" style="30" customWidth="1"/>
     <col min="3" max="3" width="75.28515625" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
     <col min="5" max="5" width="42.42578125" customWidth="1"/>
@@ -1534,11 +1584,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="41"/>
       <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1547,9 +1597,9 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="47"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1561,21 +1611,21 @@
       <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="22"/>
+      <c r="B4" s="21"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="22"/>
+      <c r="B5" s="21"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -1589,285 +1639,285 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="51">
+      <c r="B7" s="32">
         <f>SUM(B8:B13)</f>
         <v>0.10069444444444445</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="47"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="49">
+      <c r="A8" s="48">
         <v>43343</v>
       </c>
-      <c r="B8" s="48">
+      <c r="B8" s="31">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="14"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="25">
+      <c r="A9" s="49"/>
+      <c r="B9" s="24">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="14" t="s">
+      <c r="D9" s="10"/>
+      <c r="E9" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="24">
+      <c r="A10" s="49"/>
+      <c r="B10" s="23">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="14"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="24">
+      <c r="A11" s="49"/>
+      <c r="B11" s="23">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="14"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="24">
+      <c r="A12" s="49"/>
+      <c r="B12" s="23">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="14"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50"/>
-      <c r="B13" s="21">
+      <c r="A13" s="49"/>
+      <c r="B13" s="20">
         <v>3.125E-2</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="14"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="26">
         <f>SUM(B15:B23)</f>
         <v>0.1875</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="34"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="47"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35">
         <v>43347</v>
       </c>
-      <c r="B15" s="30">
+      <c r="B15" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="14" t="s">
+      <c r="D15" s="10"/>
+      <c r="E15" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
-      <c r="B16" s="24">
+      <c r="B16" s="23">
         <v>3.4722222222222224E-2</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="14"/>
-      <c r="G16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="13"/>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="36"/>
-      <c r="B17" s="24">
+      <c r="B17" s="23">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="14"/>
-      <c r="G17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="13"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
-      <c r="B18" s="24">
+      <c r="B18" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="14" t="s">
+      <c r="D18" s="10"/>
+      <c r="E18" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="38">
+      <c r="A19" s="37">
         <v>43350</v>
       </c>
-      <c r="B19" s="30">
+      <c r="B19" s="29">
         <v>3.125E-2</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="14"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
-      <c r="B20" s="30">
+      <c r="A20" s="37"/>
+      <c r="B20" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="14" t="s">
+      <c r="D20" s="10"/>
+      <c r="E20" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="30">
+      <c r="A21" s="37"/>
+      <c r="B21" s="29">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="14"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="30">
+      <c r="A22" s="37"/>
+      <c r="B22" s="29">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="14"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="39"/>
-      <c r="B23" s="24">
+      <c r="A23" s="38"/>
+      <c r="B23" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="15"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="14"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="29"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="34"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="47"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="35"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="14"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="13"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="14"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="13"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="36"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="14"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="13"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="14"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="13"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="37"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="20"/>
-      <c r="G29" s="10"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="19"/>
+      <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="40"/>
+      <c r="D30" s="33"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="41"/>
+      <c r="D31" s="34"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32"/>
-      <c r="C32" s="11"/>
+      <c r="C32" s="10"/>
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33"/>
       <c r="B33"/>
-      <c r="C33" s="11"/>
+      <c r="C33" s="10"/>
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Last add of the 14.09.2018
</commit_message>
<xml_diff>
--- a/DOC/Quentin_JDB.xlsx
+++ b/DOC/Quentin_JDB.xlsx
@@ -16,14 +16,14 @@
     <sheet name="Philippe" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Quentin!$A$1:$E$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Quentin!$A$1:$E$38</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -133,10 +133,28 @@
     <t xml:space="preserve">Ecriture des scénarios </t>
   </si>
   <si>
-    <t>Relecture du CDC et ajout / réecriture / suppression de différentes parties</t>
-  </si>
-  <si>
     <t>Certains points ne sont pas claire, ou innutile, ou manquant. Essayons de prendre le point de vue le plus claire et utile pour le client</t>
+  </si>
+  <si>
+    <t>Relécture du CDC et ajout / réecriture / suppression de différentes parties</t>
+  </si>
+  <si>
+    <t>Relécture et correction des fautes du CDC, Ajout et suppréssion de points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discution avec Philippe sur plusieurs points </t>
+  </si>
+  <si>
+    <t>Nommez  le client dans la doc ? (non). Plusieurs changement de fonctionnalités (innutiles, redondante ou pas néccessaire)</t>
+  </si>
+  <si>
+    <t>Mise en place finale du CDC en pdf</t>
+  </si>
+  <si>
+    <t>Soucis de version avec github, réglage avec Philippe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecriture de nouveaux use-case </t>
   </si>
 </sst>
 </file>
@@ -437,65 +455,65 @@
     <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -810,10 +828,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I122"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,11 +845,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="41"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="44"/>
       <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
@@ -840,9 +858,9 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="44"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="47"/>
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
@@ -889,9 +907,9 @@
         <f>SUM(B8:B13)</f>
         <v>0.10069444444444445</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="47"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="39"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="48">
@@ -972,9 +990,9 @@
         <f>SUM(B15:B23)</f>
         <v>0.1875</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="47"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
@@ -1031,7 +1049,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="37">
+      <c r="A19" s="40">
         <v>43350</v>
       </c>
       <c r="B19" s="29">
@@ -1044,7 +1062,7 @@
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="37"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1057,7 +1075,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="29">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1068,7 +1086,7 @@
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="29">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1079,7 +1097,7 @@
       <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="38"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1095,9 +1113,9 @@
         <f>SUM(B25:B29)</f>
         <v>9.375E-2</v>
       </c>
-      <c r="C24" s="45"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="47"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="39"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
     </row>
@@ -1112,7 +1130,7 @@
         <v>32</v>
       </c>
       <c r="D25" s="16"/>
-      <c r="E25" s="13"/>
+      <c r="E25" s="33"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
     </row>
@@ -1129,7 +1147,7 @@
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
     </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="36"/>
       <c r="B27" s="24">
         <v>1.0416666666666666E-2</v>
@@ -1137,9 +1155,9 @@
       <c r="C27" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="50" t="s">
-        <v>37</v>
+      <c r="D27" s="16"/>
+      <c r="E27" s="34" t="s">
+        <v>36</v>
       </c>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -1152,106 +1170,138 @@
       <c r="C28" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="15"/>
-      <c r="E28" s="50"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="34"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="52"/>
-      <c r="B29" s="25">
+      <c r="A29" s="36"/>
+      <c r="B29" s="24">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="C29" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="51"/>
+      <c r="C29" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="16"/>
+      <c r="E29" s="34"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30"/>
-      <c r="B30"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="33"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="34"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="40">
+        <v>43357</v>
+      </c>
+      <c r="B30" s="24">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="16"/>
+      <c r="E30" s="13"/>
+      <c r="G30" s="9"/>
+    </row>
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="40"/>
+      <c r="B31" s="24">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="16"/>
+      <c r="E31" s="34" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34"/>
-      <c r="B34"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="40"/>
+      <c r="B32" s="24">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="15"/>
+      <c r="E32" s="34"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="40"/>
+      <c r="B33" s="24">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="15"/>
+      <c r="E33" s="34"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="41"/>
+      <c r="B34" s="25">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="17"/>
+      <c r="E34" s="19"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35"/>
       <c r="B35"/>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36"/>
-      <c r="B36"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+    </row>
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37"/>
       <c r="B37"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38"/>
       <c r="B38"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39"/>
       <c r="B39"/>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40"/>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41"/>
       <c r="B41"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42"/>
       <c r="B42"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43"/>
       <c r="B43"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44"/>
       <c r="B44"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45"/>
       <c r="B45"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46"/>
       <c r="B46"/>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47"/>
       <c r="B47"/>
     </row>
-    <row r="48" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48"/>
       <c r="B48"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49"/>
       <c r="B49"/>
     </row>
@@ -1287,11 +1337,11 @@
       <c r="A57"/>
       <c r="B57"/>
     </row>
-    <row r="58" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58"/>
       <c r="B58"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59"/>
       <c r="B59"/>
     </row>
@@ -1327,11 +1377,11 @@
       <c r="A67"/>
       <c r="B67"/>
     </row>
-    <row r="68" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68"/>
       <c r="B68"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69"/>
       <c r="B69"/>
     </row>
@@ -1351,11 +1401,11 @@
       <c r="A73"/>
       <c r="B73"/>
     </row>
-    <row r="74" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74"/>
       <c r="B74"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75"/>
       <c r="B75"/>
     </row>
@@ -1547,9 +1597,12 @@
       <c r="A122"/>
       <c r="B122"/>
     </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123"/>
+      <c r="B123"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="D30:D31"/>
+  <mergeCells count="11">
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A19:A23"/>
     <mergeCell ref="A1:C2"/>
@@ -1559,6 +1612,8 @@
     <mergeCell ref="E27:E29"/>
     <mergeCell ref="A25:A29"/>
     <mergeCell ref="C24:E24"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="E31:E33"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="68" fitToHeight="5" orientation="landscape" r:id="rId1"/>
@@ -1584,11 +1639,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="41"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="44"/>
       <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1597,9 +1652,9 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="44"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="47"/>
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1646,9 +1701,9 @@
         <f>SUM(B8:B13)</f>
         <v>0.10069444444444445</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="47"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="39"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="48">
@@ -1728,9 +1783,9 @@
         <f>SUM(B15:B23)</f>
         <v>0.1875</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="47"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
@@ -1787,7 +1842,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="37">
+      <c r="A19" s="40">
         <v>43350</v>
       </c>
       <c r="B19" s="29">
@@ -1800,7 +1855,7 @@
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="37"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1813,7 +1868,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="29">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1824,7 +1879,7 @@
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="29">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1835,7 +1890,7 @@
       <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="38"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1848,9 +1903,9 @@
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="28"/>
       <c r="B24" s="26"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="47"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="39"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
     </row>
@@ -1889,7 +1944,7 @@
       <c r="E28" s="13"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="52"/>
+      <c r="A29" s="50"/>
       <c r="B29" s="25"/>
       <c r="C29" s="18"/>
       <c r="D29" s="17"/>
@@ -1900,13 +1955,13 @@
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="33"/>
+      <c r="D30" s="51"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="34"/>
+      <c r="D31" s="52"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32"/>

</xml_diff>

<commit_message>
order the img of the documentation files
Add folders and hierarchy organisation
</commit_message>
<xml_diff>
--- a/DOC/Quentin_JDB.xlsx
+++ b/DOC/Quentin_JDB.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
   <si>
     <t>Date</t>
   </si>
@@ -209,6 +209,27 @@
   </si>
   <si>
     <t>Compréhension du site et de son fonctionnement, création du premier sprint</t>
+  </si>
+  <si>
+    <t>Semaie 6</t>
+  </si>
+  <si>
+    <t>Lecture de documentations sur LINQ</t>
+  </si>
+  <si>
+    <t>Semble être efficace</t>
+  </si>
+  <si>
+    <t>mise en place de l'écriture dans un fichier</t>
+  </si>
+  <si>
+    <t>récupération des données passées</t>
+  </si>
+  <si>
+    <t>9h</t>
+  </si>
+  <si>
+    <t>questionnaire kali T</t>
   </si>
 </sst>
 </file>
@@ -512,63 +533,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -576,6 +540,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -893,7 +914,7 @@
   <dimension ref="A1:I123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,12 +990,12 @@
         <f>SUM(B8:B13)</f>
         <v>0.10069444444444445</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="36"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="50"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="48">
+      <c r="A8" s="51">
         <v>43343</v>
       </c>
       <c r="B8" s="31">
@@ -987,7 +1008,7 @@
       <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
+      <c r="A9" s="52"/>
       <c r="B9" s="24">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1001,7 +1022,7 @@
       <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
+      <c r="A10" s="52"/>
       <c r="B10" s="23">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1012,7 +1033,7 @@
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
+      <c r="A11" s="52"/>
       <c r="B11" s="23">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1023,7 +1044,7 @@
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
+      <c r="A12" s="52"/>
       <c r="B12" s="23">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1034,7 +1055,7 @@
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
+      <c r="A13" s="52"/>
       <c r="B13" s="20">
         <v>3.125E-2</v>
       </c>
@@ -1052,14 +1073,14 @@
         <f>SUM(B15:B23)</f>
         <v>0.1875</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="36"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="50"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37">
+      <c r="A15" s="38">
         <v>43347</v>
       </c>
       <c r="B15" s="29">
@@ -1074,7 +1095,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="23">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1086,7 +1107,7 @@
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="23">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1098,7 +1119,7 @@
       <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="38"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1111,7 +1132,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="39">
+      <c r="A19" s="40">
         <v>43350</v>
       </c>
       <c r="B19" s="29">
@@ -1124,7 +1145,7 @@
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1137,7 +1158,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="29">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1148,7 +1169,7 @@
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="29">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1159,7 +1180,7 @@
       <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="40"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1177,14 +1198,14 @@
         <f>SUM(B25:B29)</f>
         <v>9.375E-2</v>
       </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="36"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="50"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="37">
+      <c r="A25" s="38">
         <v>43354</v>
       </c>
       <c r="B25" s="24">
@@ -1199,7 +1220,7 @@
       <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="38"/>
+      <c r="A26" s="39"/>
       <c r="B26" s="24">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1212,7 +1233,7 @@
       <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="38"/>
+      <c r="A27" s="39"/>
       <c r="B27" s="24">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1220,14 +1241,14 @@
         <v>34</v>
       </c>
       <c r="D27" s="16"/>
-      <c r="E27" s="41" t="s">
+      <c r="E27" s="53" t="s">
         <v>36</v>
       </c>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
+      <c r="A28" s="39"/>
       <c r="B28" s="24">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1235,10 +1256,10 @@
         <v>35</v>
       </c>
       <c r="D28" s="16"/>
-      <c r="E28" s="41"/>
+      <c r="E28" s="53"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
+      <c r="A29" s="39"/>
       <c r="B29" s="24">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1246,11 +1267,11 @@
         <v>37</v>
       </c>
       <c r="D29" s="16"/>
-      <c r="E29" s="41"/>
+      <c r="E29" s="53"/>
       <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="39">
+      <c r="A30" s="40">
         <v>43357</v>
       </c>
       <c r="B30" s="24">
@@ -1264,7 +1285,7 @@
       <c r="G30" s="9"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="39"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="24">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1272,12 +1293,12 @@
         <v>39</v>
       </c>
       <c r="D31" s="16"/>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="53" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="39"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="24">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1285,10 +1306,10 @@
         <v>43</v>
       </c>
       <c r="D32" s="15"/>
-      <c r="E32" s="41"/>
+      <c r="E32" s="53"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="39"/>
+      <c r="A33" s="40"/>
       <c r="B33" s="24">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1296,10 +1317,10 @@
         <v>42</v>
       </c>
       <c r="D33" s="15"/>
-      <c r="E33" s="41"/>
+      <c r="E33" s="53"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="40"/>
+      <c r="A34" s="41"/>
       <c r="B34" s="25">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1314,11 +1335,11 @@
         <v>46</v>
       </c>
       <c r="B35" s="26"/>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="35"/>
-      <c r="E35" s="36"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="50"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="28" t="s">
@@ -1328,12 +1349,12 @@
         <f>SUM(B37:B47)</f>
         <v>0.1875</v>
       </c>
-      <c r="C36" s="34"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="36"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="50"/>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="37">
+      <c r="A37" s="38">
         <v>43368</v>
       </c>
       <c r="B37" s="24">
@@ -1350,7 +1371,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="38"/>
+      <c r="A38" s="39"/>
       <c r="B38" s="24">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1361,7 +1382,7 @@
       <c r="E38" s="13"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="38"/>
+      <c r="A39" s="39"/>
       <c r="B39" s="24">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1374,7 +1395,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="38"/>
+      <c r="A40" s="39"/>
       <c r="B40" s="24">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1385,7 +1406,7 @@
       <c r="E40" s="13"/>
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="38"/>
+      <c r="A41" s="39"/>
       <c r="B41" s="24">
         <v>3.472222222222222E-3</v>
       </c>
@@ -1396,7 +1417,7 @@
       <c r="E41" s="13"/>
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="38">
+      <c r="A42" s="39">
         <v>43371</v>
       </c>
       <c r="B42" s="24">
@@ -1409,7 +1430,7 @@
       <c r="E42" s="13"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="38"/>
+      <c r="A43" s="39"/>
       <c r="B43" s="24">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1422,7 +1443,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="38"/>
+      <c r="A44" s="39"/>
       <c r="B44" s="24">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1433,7 +1454,7 @@
       <c r="E44" s="13"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="38"/>
+      <c r="A45" s="39"/>
       <c r="B45" s="24">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1444,7 +1465,7 @@
       <c r="E45" s="13"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="38"/>
+      <c r="A46" s="39"/>
       <c r="B46" s="24">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1455,81 +1476,140 @@
       <c r="E46" s="13"/>
     </row>
     <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="40"/>
-      <c r="B47" s="56">
+      <c r="A47" s="41"/>
+      <c r="B47" s="37">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="C47" s="53" t="s">
+      <c r="C47" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D47" s="54"/>
-      <c r="E47" s="55"/>
-    </row>
-    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48"/>
-      <c r="B48"/>
-    </row>
-    <row r="49" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49"/>
-      <c r="B49"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50"/>
-      <c r="B50"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51"/>
-      <c r="B51" s="9"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52"/>
-      <c r="B52"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53"/>
-      <c r="B53"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54"/>
-      <c r="B54"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55"/>
-      <c r="B55"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56"/>
-      <c r="B56"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57"/>
-      <c r="B57"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58"/>
-      <c r="B58"/>
-    </row>
-    <row r="59" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59"/>
-      <c r="B59"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D47" s="35"/>
+      <c r="E47" s="36"/>
+    </row>
+    <row r="48" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="26">
+        <f>SUM(B49:B59)</f>
+        <v>4.1666666666666671E-2</v>
+      </c>
+      <c r="C48" s="48"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="50"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="38">
+        <v>43375</v>
+      </c>
+      <c r="B49" s="24">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="16"/>
+      <c r="E49" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="39"/>
+      <c r="B50" s="24">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50" s="16"/>
+      <c r="E50" s="13"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="39"/>
+      <c r="B51" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D51" s="16"/>
+      <c r="E51" s="13"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="39"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" s="16"/>
+      <c r="E52" s="13"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="39"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="13"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="39"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="13"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="39"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="13"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="39"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="13"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="39"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="13"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="39"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="13"/>
+    </row>
+    <row r="59" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="41"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="36"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60"/>
       <c r="B60"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61"/>
       <c r="B61"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62"/>
       <c r="B62"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63"/>
       <c r="B63"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64"/>
       <c r="B64"/>
     </row>
@@ -1770,22 +1850,25 @@
       <c r="B123"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="18">
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A54:A59"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A42:A47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="E31:E33"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A19:A23"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="A8:A13"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A42:A47"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="68" fitToHeight="5" orientation="landscape" r:id="rId1"/>
@@ -1873,12 +1956,12 @@
         <f>SUM(B8:B13)</f>
         <v>0.10069444444444445</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="36"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="50"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="48">
+      <c r="A8" s="51">
         <v>43343</v>
       </c>
       <c r="B8" s="31">
@@ -1891,7 +1974,7 @@
       <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
+      <c r="A9" s="52"/>
       <c r="B9" s="24">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1904,7 +1987,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
+      <c r="A10" s="52"/>
       <c r="B10" s="23">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1915,7 +1998,7 @@
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
+      <c r="A11" s="52"/>
       <c r="B11" s="23">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1926,7 +2009,7 @@
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
+      <c r="A12" s="52"/>
       <c r="B12" s="23">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1937,7 +2020,7 @@
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
+      <c r="A13" s="52"/>
       <c r="B13" s="20">
         <v>3.125E-2</v>
       </c>
@@ -1955,14 +2038,14 @@
         <f>SUM(B15:B23)</f>
         <v>0.1875</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="36"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="50"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37">
+      <c r="A15" s="38">
         <v>43347</v>
       </c>
       <c r="B15" s="29">
@@ -1977,7 +2060,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="23">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1989,7 +2072,7 @@
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="23">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -2001,7 +2084,7 @@
       <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="38"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -2014,7 +2097,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="39">
+      <c r="A19" s="40">
         <v>43350</v>
       </c>
       <c r="B19" s="29">
@@ -2027,7 +2110,7 @@
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -2040,7 +2123,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="29">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -2051,7 +2134,7 @@
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="29">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -2062,7 +2145,7 @@
       <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="40"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -2075,14 +2158,14 @@
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="28"/>
       <c r="B24" s="26"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="36"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="50"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="37"/>
+      <c r="A25" s="38"/>
       <c r="B25" s="24"/>
       <c r="C25" s="15"/>
       <c r="D25" s="16"/>
@@ -2091,7 +2174,7 @@
       <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="38"/>
+      <c r="A26" s="39"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -2100,7 +2183,7 @@
       <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="38"/>
+      <c r="A27" s="39"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="15"/>
@@ -2109,14 +2192,14 @@
       <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
+      <c r="A28" s="39"/>
       <c r="B28" s="24"/>
       <c r="C28" s="16"/>
       <c r="D28" s="15"/>
       <c r="E28" s="13"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="25"/>
       <c r="C29" s="18"/>
       <c r="D29" s="17"/>
@@ -2127,13 +2210,13 @@
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="51"/>
+      <c r="D30" s="55"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="52"/>
+      <c r="D31" s="56"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32"/>

</xml_diff>

<commit_message>
add day to 20.11.2018
</commit_message>
<xml_diff>
--- a/DOC/Quentin_JDB.xlsx
+++ b/DOC/Quentin_JDB.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="125">
   <si>
     <t>Date</t>
   </si>
@@ -328,9 +328,6 @@
     <t>Uniquement 2 périodes cette semaines</t>
   </si>
   <si>
-    <t>oupsi doupsi</t>
-  </si>
-  <si>
     <t>Création et mise en place du trello</t>
   </si>
   <si>
@@ -347,6 +344,60 @@
   </si>
   <si>
     <t xml:space="preserve">datetime.now et pas .today </t>
+  </si>
+  <si>
+    <t>Discution sur les portes ouvertes, sur la présentation à faire</t>
+  </si>
+  <si>
+    <t>Retard de 50m</t>
+  </si>
+  <si>
+    <t>Absence</t>
+  </si>
+  <si>
+    <t>jdb</t>
+  </si>
+  <si>
+    <t>Semaine 9</t>
+  </si>
+  <si>
+    <t>Semaine 10</t>
+  </si>
+  <si>
+    <t>PB à la banque</t>
+  </si>
+  <si>
+    <t>Reglage d'un bug sur le stockage de la recherche</t>
+  </si>
+  <si>
+    <t>Problème dans la boucle</t>
+  </si>
+  <si>
+    <t>Il stockas nfois la ligne 1</t>
+  </si>
+  <si>
+    <t>bug d'ouvertur de fichier dans l'explorer et avec le logiciel par défaut</t>
+  </si>
+  <si>
+    <t>Codage à deux pour la classe log</t>
+  </si>
+  <si>
+    <t>explication par filipe</t>
+  </si>
+  <si>
+    <t>Discution avec Filipe et M.Hurni sur la structure de programme et des changements à faire</t>
+  </si>
+  <si>
+    <t>Il faut que notre code soit modulable</t>
+  </si>
+  <si>
+    <t>Création du fichier de structure de programme et modification de celui-ci</t>
+  </si>
+  <si>
+    <t>Codae de la classe loghandler</t>
+  </si>
+  <si>
+    <t>Semaine 11</t>
   </si>
 </sst>
 </file>
@@ -565,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -671,17 +722,28 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -741,6 +803,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1055,16 +1120,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I119"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="21"/>
-    <col min="2" max="2" width="9.5703125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="21" customWidth="1"/>
     <col min="3" max="3" width="75.28515625" customWidth="1"/>
     <col min="4" max="4" width="43.42578125" customWidth="1"/>
     <col min="5" max="5" width="44" customWidth="1"/>
@@ -1072,11 +1137,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="62"/>
       <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1085,9 +1150,9 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="62"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="65"/>
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1103,12 +1168,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="21"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="21"/>
-    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>0</v>
@@ -1134,12 +1194,12 @@
         <f>SUM(B8:B13)</f>
         <v>0.10069444444444445</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="53"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="56"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="63">
+      <c r="A8" s="66">
         <v>43343</v>
       </c>
       <c r="B8" s="31">
@@ -1152,7 +1212,7 @@
       <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="64"/>
+      <c r="A9" s="67"/>
       <c r="B9" s="24">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1166,7 +1226,7 @@
       <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="64"/>
+      <c r="A10" s="67"/>
       <c r="B10" s="23">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1177,7 +1237,7 @@
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="64"/>
+      <c r="A11" s="67"/>
       <c r="B11" s="23">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1188,7 +1248,7 @@
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="64"/>
+      <c r="A12" s="67"/>
       <c r="B12" s="23">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1199,7 +1259,7 @@
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="64"/>
+      <c r="A13" s="67"/>
       <c r="B13" s="20">
         <v>3.125E-2</v>
       </c>
@@ -1217,14 +1277,14 @@
         <f>SUM(B15:B23)</f>
         <v>0.1875</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="53"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="56"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="54">
+      <c r="A15" s="57">
         <v>43347</v>
       </c>
       <c r="B15" s="29">
@@ -1239,7 +1299,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="23">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1251,7 +1311,7 @@
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="23">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1263,7 +1323,7 @@
       <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1276,7 +1336,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="47">
+      <c r="A19" s="48">
         <v>43350</v>
       </c>
       <c r="B19" s="29">
@@ -1289,7 +1349,7 @@
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1302,7 +1362,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
+      <c r="A21" s="48"/>
       <c r="B21" s="29">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1313,7 +1373,7 @@
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="29">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1324,7 +1384,7 @@
       <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="46"/>
+      <c r="A23" s="49"/>
       <c r="B23" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1342,14 +1402,14 @@
         <f>SUM(B25:B29)</f>
         <v>9.375E-2</v>
       </c>
-      <c r="C24" s="51"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="53"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="56"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="54">
+      <c r="A25" s="57">
         <v>43354</v>
       </c>
       <c r="B25" s="24">
@@ -1364,7 +1424,7 @@
       <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
+      <c r="A26" s="50"/>
       <c r="B26" s="24">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1377,7 +1437,7 @@
       <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="45"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="24">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1385,14 +1445,14 @@
         <v>34</v>
       </c>
       <c r="D27" s="16"/>
-      <c r="E27" s="56" t="s">
+      <c r="E27" s="59" t="s">
         <v>36</v>
       </c>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="45"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="24">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1400,10 +1460,10 @@
         <v>35</v>
       </c>
       <c r="D28" s="16"/>
-      <c r="E28" s="56"/>
+      <c r="E28" s="59"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="45"/>
+      <c r="A29" s="50"/>
       <c r="B29" s="24">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1411,11 +1471,11 @@
         <v>37</v>
       </c>
       <c r="D29" s="16"/>
-      <c r="E29" s="56"/>
+      <c r="E29" s="59"/>
       <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="47">
+      <c r="A30" s="48">
         <v>43357</v>
       </c>
       <c r="B30" s="24">
@@ -1429,7 +1489,7 @@
       <c r="G30" s="9"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
+      <c r="A31" s="48"/>
       <c r="B31" s="24">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1437,12 +1497,12 @@
         <v>39</v>
       </c>
       <c r="D31" s="16"/>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="59" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
+      <c r="A32" s="48"/>
       <c r="B32" s="24">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1450,10 +1510,10 @@
         <v>43</v>
       </c>
       <c r="D32" s="15"/>
-      <c r="E32" s="56"/>
+      <c r="E32" s="59"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
+      <c r="A33" s="48"/>
       <c r="B33" s="24">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1461,10 +1521,10 @@
         <v>42</v>
       </c>
       <c r="D33" s="15"/>
-      <c r="E33" s="56"/>
+      <c r="E33" s="59"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="46"/>
+      <c r="A34" s="49"/>
       <c r="B34" s="25">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1479,11 +1539,11 @@
         <v>46</v>
       </c>
       <c r="B35" s="26"/>
-      <c r="C35" s="51" t="s">
+      <c r="C35" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="52"/>
-      <c r="E35" s="53"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="56"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="28" t="s">
@@ -1493,12 +1553,12 @@
         <f>SUM(B37:B47)</f>
         <v>0.1875</v>
       </c>
-      <c r="C36" s="51"/>
-      <c r="D36" s="52"/>
-      <c r="E36" s="53"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="56"/>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="54">
+      <c r="A37" s="57">
         <v>43368</v>
       </c>
       <c r="B37" s="24">
@@ -1515,7 +1575,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="45"/>
+      <c r="A38" s="50"/>
       <c r="B38" s="24">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1526,7 +1586,7 @@
       <c r="E38" s="13"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="45"/>
+      <c r="A39" s="50"/>
       <c r="B39" s="24">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1539,7 +1599,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="45"/>
+      <c r="A40" s="50"/>
       <c r="B40" s="24">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1550,7 +1610,7 @@
       <c r="E40" s="13"/>
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="45"/>
+      <c r="A41" s="50"/>
       <c r="B41" s="24">
         <v>3.472222222222222E-3</v>
       </c>
@@ -1561,7 +1621,7 @@
       <c r="E41" s="13"/>
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="45">
+      <c r="A42" s="50">
         <v>43371</v>
       </c>
       <c r="B42" s="24">
@@ -1574,7 +1634,7 @@
       <c r="E42" s="13"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="45"/>
+      <c r="A43" s="50"/>
       <c r="B43" s="24">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1587,7 +1647,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="45"/>
+      <c r="A44" s="50"/>
       <c r="B44" s="24">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1598,7 +1658,7 @@
       <c r="E44" s="13"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="45"/>
+      <c r="A45" s="50"/>
       <c r="B45" s="24">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1609,7 +1669,7 @@
       <c r="E45" s="13"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="45"/>
+      <c r="A46" s="50"/>
       <c r="B46" s="24">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1620,7 +1680,7 @@
       <c r="E46" s="13"/>
     </row>
     <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="46"/>
+      <c r="A47" s="49"/>
       <c r="B47" s="38">
         <v>3.472222222222222E-3</v>
       </c>
@@ -1638,12 +1698,12 @@
         <f>SUM(B49:B55)</f>
         <v>9.3750000000000014E-2</v>
       </c>
-      <c r="C48" s="51"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="53"/>
+      <c r="C48" s="54"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="56"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="54">
+      <c r="A49" s="57">
         <v>43375</v>
       </c>
       <c r="B49" s="24">
@@ -1658,7 +1718,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="45"/>
+      <c r="A50" s="50"/>
       <c r="B50" s="24">
         <v>2.4305555555555556E-2</v>
       </c>
@@ -1671,7 +1731,7 @@
       <c r="E50" s="13"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="45"/>
+      <c r="A51" s="50"/>
       <c r="B51" s="24">
         <v>3.472222222222222E-3</v>
       </c>
@@ -1682,7 +1742,7 @@
       <c r="E51" s="13"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="45"/>
+      <c r="A52" s="50"/>
       <c r="B52" s="24">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1693,7 +1753,7 @@
       <c r="E52" s="13"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="45"/>
+      <c r="A53" s="50"/>
       <c r="B53" s="24">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1701,12 +1761,12 @@
         <v>65</v>
       </c>
       <c r="D53" s="16"/>
-      <c r="E53" s="55" t="s">
+      <c r="E53" s="58" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="45"/>
+      <c r="A54" s="50"/>
       <c r="B54" s="24">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1714,7 +1774,7 @@
         <v>63</v>
       </c>
       <c r="D54" s="16"/>
-      <c r="E54" s="55"/>
+      <c r="E54" s="58"/>
     </row>
     <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="34">
@@ -1735,12 +1795,12 @@
         <f>SUM(B57:B65)</f>
         <v>0.1875</v>
       </c>
-      <c r="C56" s="51"/>
-      <c r="D56" s="52"/>
-      <c r="E56" s="53"/>
+      <c r="C56" s="54"/>
+      <c r="D56" s="55"/>
+      <c r="E56" s="56"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="54">
+      <c r="A57" s="57">
         <v>43382</v>
       </c>
       <c r="B57" s="24">
@@ -1753,7 +1813,7 @@
       <c r="E57" s="13"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="45"/>
+      <c r="A58" s="50"/>
       <c r="B58" s="24">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1764,7 +1824,7 @@
       <c r="E58" s="13"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="45"/>
+      <c r="A59" s="50"/>
       <c r="B59" s="24">
         <v>5.2083333333333336E-2</v>
       </c>
@@ -1775,7 +1835,7 @@
       <c r="E59" s="13"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="45"/>
+      <c r="A60" s="50"/>
       <c r="B60" s="24">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1788,7 +1848,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="45"/>
+      <c r="A61" s="50"/>
       <c r="B61" s="24">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1801,7 +1861,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="45">
+      <c r="A62" s="50">
         <v>43385</v>
       </c>
       <c r="B62" s="24">
@@ -1814,7 +1874,7 @@
       <c r="E62" s="13"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="45"/>
+      <c r="A63" s="50"/>
       <c r="B63" s="24">
         <v>3.125E-2</v>
       </c>
@@ -1827,7 +1887,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="45"/>
+      <c r="A64" s="50"/>
       <c r="B64" s="24">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1838,7 +1898,7 @@
       <c r="E64" s="13"/>
     </row>
     <row r="65" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="46"/>
+      <c r="A65" s="49"/>
       <c r="B65" s="38">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1854,19 +1914,19 @@
       <c r="A66" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="B66" s="43">
-        <f ca="1">SUM(B66:B73)</f>
-        <v>0</v>
-      </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="49"/>
-      <c r="E66" s="50"/>
+      <c r="B66" s="45">
+        <f>SUM(B67:B73)</f>
+        <v>0.15624999999999997</v>
+      </c>
+      <c r="C66" s="51"/>
+      <c r="D66" s="52"/>
+      <c r="E66" s="53"/>
     </row>
     <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="47">
+      <c r="A67" s="48">
         <v>43404</v>
       </c>
-      <c r="B67" s="9">
+      <c r="B67" s="29">
         <v>2.4305555555555556E-2</v>
       </c>
       <c r="C67" t="s">
@@ -1880,8 +1940,8 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="47"/>
-      <c r="B68" s="9">
+      <c r="A68" s="48"/>
+      <c r="B68" s="29">
         <v>3.8194444444444441E-2</v>
       </c>
       <c r="C68" s="40" t="s">
@@ -1895,10 +1955,10 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="45">
+      <c r="A69" s="50">
         <v>43406</v>
       </c>
-      <c r="B69" s="9">
+      <c r="B69" s="29">
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="C69" t="s">
@@ -1907,8 +1967,8 @@
       <c r="E69" s="5"/>
     </row>
     <row r="70" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="45"/>
-      <c r="B70" s="9">
+      <c r="A70" s="50"/>
+      <c r="B70" s="29">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="C70" t="s">
@@ -1920,8 +1980,8 @@
       <c r="E70" s="5"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="45"/>
-      <c r="B71" s="9">
+      <c r="A71" s="50"/>
+      <c r="B71" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="C71" t="s">
@@ -1930,8 +1990,8 @@
       <c r="E71" s="5"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="45"/>
-      <c r="B72" s="9">
+      <c r="A72" s="50"/>
+      <c r="B72" s="29">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="C72" t="s">
@@ -1940,8 +2000,8 @@
       <c r="E72" s="5"/>
     </row>
     <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="46"/>
-      <c r="B73" s="44">
+      <c r="A73" s="49"/>
+      <c r="B73" s="46">
         <v>1.7361111111111112E-2</v>
       </c>
       <c r="C73" s="36" t="s">
@@ -1952,224 +2012,285 @@
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74"/>
-      <c r="B74"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75"/>
-      <c r="B75"/>
-      <c r="C75" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76"/>
-      <c r="B76" s="9">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="C76" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77"/>
-      <c r="B77" s="9">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C77" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78"/>
-      <c r="B78" s="9">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C78" t="s">
-        <v>104</v>
-      </c>
-      <c r="D78" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79"/>
-      <c r="B79" s="9">
-        <v>2.4305555555555556E-2</v>
-      </c>
-      <c r="C79" t="s">
-        <v>105</v>
-      </c>
-      <c r="D79" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80"/>
-      <c r="B80"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81"/>
-      <c r="B81" s="9">
+    <row r="74" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B74" s="45">
         <f>SUM(B76:B79)</f>
         <v>9.3749999999999986E-2</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82"/>
-      <c r="B82"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83"/>
-      <c r="B83"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84"/>
-      <c r="B84"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85"/>
-      <c r="B85"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86"/>
-      <c r="B86"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87"/>
-      <c r="B87"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88"/>
-      <c r="B88"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89"/>
-      <c r="B89"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90"/>
-      <c r="B90"/>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74" s="51"/>
+      <c r="D74" s="52"/>
+      <c r="E74" s="53"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="43">
+        <v>43410</v>
+      </c>
+      <c r="C75" t="s">
+        <v>109</v>
+      </c>
+      <c r="E75" s="5"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="50">
+        <v>43413</v>
+      </c>
+      <c r="B76" s="47">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="C76" t="s">
+        <v>101</v>
+      </c>
+      <c r="E76" s="5"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="50"/>
+      <c r="B77" s="47">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C77" t="s">
+        <v>102</v>
+      </c>
+      <c r="E77" s="5"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="50"/>
+      <c r="B78" s="47">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C78" t="s">
+        <v>103</v>
+      </c>
+      <c r="D78" t="s">
+        <v>106</v>
+      </c>
+      <c r="E78" s="5"/>
+    </row>
+    <row r="79" spans="1:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="49"/>
+      <c r="B79" s="46">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="C79" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D79" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="E79" s="37"/>
+    </row>
+    <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B80" s="45">
+        <f>SUM(B82:B85)</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="C80" s="51"/>
+      <c r="D80" s="52"/>
+      <c r="E80" s="53"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="43">
+        <v>43419</v>
+      </c>
+      <c r="B81" s="29">
+        <v>9.375E-2</v>
+      </c>
+      <c r="C81" t="s">
+        <v>107</v>
+      </c>
+      <c r="E81" s="5"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="48">
+        <v>43420</v>
+      </c>
+      <c r="C82" t="s">
+        <v>108</v>
+      </c>
+      <c r="D82" t="s">
+        <v>113</v>
+      </c>
+      <c r="E82" s="5"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="48"/>
+      <c r="B83" s="29">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C83" t="s">
+        <v>110</v>
+      </c>
+      <c r="E83" s="5"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="48"/>
+      <c r="B84" s="29">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="C84" t="s">
+        <v>114</v>
+      </c>
+      <c r="D84" t="s">
+        <v>115</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="48"/>
+      <c r="B85" s="29">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C85" t="s">
+        <v>117</v>
+      </c>
+      <c r="E85" s="5"/>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B86" s="45">
+        <f>SUM(B87:B90)</f>
+        <v>9.3749999999999986E-2</v>
+      </c>
+      <c r="C86" s="51"/>
+      <c r="D86" s="52"/>
+      <c r="E86" s="53"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="71"/>
+      <c r="B87" s="29">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C87" t="s">
+        <v>118</v>
+      </c>
+      <c r="D87" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="71"/>
+      <c r="B88" s="29">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C88" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="71"/>
+      <c r="B89" s="29">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C89" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="E89" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="71"/>
+      <c r="B90" s="29">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C90" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91"/>
-      <c r="B91"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92"/>
-      <c r="B92"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93"/>
-      <c r="B93"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94"/>
-      <c r="B94"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95"/>
-      <c r="B95"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96"/>
-      <c r="B96"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97"/>
-      <c r="B97"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98"/>
-      <c r="B98"/>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99"/>
-      <c r="B99"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100"/>
-      <c r="B100"/>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101"/>
-      <c r="B101"/>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102"/>
-      <c r="B102"/>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103"/>
-      <c r="B103"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104"/>
-      <c r="B104"/>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105"/>
-      <c r="B105"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106"/>
-      <c r="B106"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107"/>
-      <c r="B107"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108"/>
-      <c r="B108"/>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109"/>
-      <c r="B109"/>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110"/>
-      <c r="B110"/>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111"/>
-      <c r="B111"/>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112"/>
-      <c r="B112"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113"/>
-      <c r="B113"/>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114"/>
-      <c r="B114"/>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115"/>
-      <c r="B115"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116"/>
-      <c r="B116"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117"/>
-      <c r="B117"/>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118"/>
-      <c r="B118"/>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119"/>
-      <c r="B119"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="30">
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="C86:E86"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A19:A23"/>
     <mergeCell ref="A1:C2"/>
@@ -2181,6 +2302,8 @@
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="E31:E33"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="A57:A61"/>
     <mergeCell ref="A49:A54"/>
     <mergeCell ref="E53:E54"/>
     <mergeCell ref="C35:E35"/>
@@ -2188,12 +2311,14 @@
     <mergeCell ref="A37:A41"/>
     <mergeCell ref="A42:A47"/>
     <mergeCell ref="C48:E48"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C80:E80"/>
     <mergeCell ref="A62:A65"/>
     <mergeCell ref="A69:A73"/>
     <mergeCell ref="A67:A68"/>
     <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="A57:A61"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="68" fitToHeight="5" orientation="landscape" r:id="rId1"/>
@@ -2219,11 +2344,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="62"/>
       <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2232,9 +2357,9 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="62"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="65"/>
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
@@ -2281,12 +2406,12 @@
         <f>SUM(B8:B13)</f>
         <v>0.10069444444444445</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="53"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="56"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="63">
+      <c r="A8" s="66">
         <v>43343</v>
       </c>
       <c r="B8" s="31">
@@ -2299,7 +2424,7 @@
       <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="64"/>
+      <c r="A9" s="67"/>
       <c r="B9" s="24">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -2312,7 +2437,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="64"/>
+      <c r="A10" s="67"/>
       <c r="B10" s="23">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -2323,7 +2448,7 @@
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="64"/>
+      <c r="A11" s="67"/>
       <c r="B11" s="23">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -2334,7 +2459,7 @@
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="64"/>
+      <c r="A12" s="67"/>
       <c r="B12" s="23">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -2345,7 +2470,7 @@
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="64"/>
+      <c r="A13" s="67"/>
       <c r="B13" s="20">
         <v>3.125E-2</v>
       </c>
@@ -2363,14 +2488,14 @@
         <f>SUM(B15:B23)</f>
         <v>0.1875</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="53"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="56"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="54">
+      <c r="A15" s="57">
         <v>43347</v>
       </c>
       <c r="B15" s="29">
@@ -2385,7 +2510,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="23">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -2397,7 +2522,7 @@
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="23">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -2409,7 +2534,7 @@
       <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -2422,7 +2547,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="47">
+      <c r="A19" s="48">
         <v>43350</v>
       </c>
       <c r="B19" s="29">
@@ -2435,7 +2560,7 @@
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -2448,7 +2573,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
+      <c r="A21" s="48"/>
       <c r="B21" s="29">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -2459,7 +2584,7 @@
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="29">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -2470,7 +2595,7 @@
       <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="46"/>
+      <c r="A23" s="49"/>
       <c r="B23" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -2483,14 +2608,14 @@
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="28"/>
       <c r="B24" s="26"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="53"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="56"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="54"/>
+      <c r="A25" s="57"/>
       <c r="B25" s="24"/>
       <c r="C25" s="15"/>
       <c r="D25" s="16"/>
@@ -2499,7 +2624,7 @@
       <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
+      <c r="A26" s="50"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -2508,7 +2633,7 @@
       <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="45"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="15"/>
@@ -2517,14 +2642,14 @@
       <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="45"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="24"/>
       <c r="C28" s="16"/>
       <c r="D28" s="15"/>
       <c r="E28" s="13"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="65"/>
+      <c r="A29" s="68"/>
       <c r="B29" s="25"/>
       <c r="C29" s="18"/>
       <c r="D29" s="17"/>
@@ -2535,13 +2660,13 @@
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="66"/>
+      <c r="D30" s="69"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="67"/>
+      <c r="D31" s="70"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32"/>

</xml_diff>